<commit_message>
Funcionou - Começando a coletar a base
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="35">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -37,27 +37,18 @@
     <t>Agrale</t>
   </si>
   <si>
-    <t>Alfa Romeo</t>
-  </si>
-  <si>
     <t>Integra GS 1.8</t>
   </si>
   <si>
     <t>Legend 3.2/3.5</t>
   </si>
   <si>
+    <t>NSX 3.0</t>
+  </si>
+  <si>
     <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
   </si>
   <si>
-    <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
-  </si>
-  <si>
-    <t>145 Elegant 1.7/1.8 16V</t>
-  </si>
-  <si>
-    <t>145 Elegant 2.0 16V</t>
-  </si>
-  <si>
     <t>1992 Gasolina</t>
   </si>
   <si>
@@ -70,13 +61,28 @@
     <t>1997 Gasolina</t>
   </si>
   <si>
+    <t>1996 Gasolina</t>
+  </si>
+  <si>
+    <t>1995 Gasolina</t>
+  </si>
+  <si>
+    <t>1994 Gasolina</t>
+  </si>
+  <si>
+    <t>1993 Gasolina</t>
+  </si>
+  <si>
     <t>2007 Diesel</t>
   </si>
   <si>
     <t>2006 Diesel</t>
   </si>
   <si>
-    <t>1999 Gasolina</t>
+    <t>2005 Diesel</t>
+  </si>
+  <si>
+    <t>2004 Diesel</t>
   </si>
   <si>
     <t>038003-2</t>
@@ -85,15 +91,12 @@
     <t>038002-4</t>
   </si>
   <si>
+    <t>038001-6</t>
+  </si>
+  <si>
     <t>060001-6</t>
   </si>
   <si>
-    <t>006009-7</t>
-  </si>
-  <si>
-    <t>006001-1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 11120.00</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t xml:space="preserve"> 14248.00</t>
   </si>
   <si>
+    <t xml:space="preserve"> 33464.00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 48348.00</t>
   </si>
   <si>
@@ -112,16 +118,7 @@
     <t xml:space="preserve"> 43449.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 27043.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 21667.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 21690.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17716.00</t>
+    <t xml:space="preserve"> 36830.00</t>
   </si>
 </sst>
 </file>
@@ -479,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,16 +504,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -524,16 +521,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -541,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -558,30 +555,30 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -589,95 +586,95 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -686,15 +683,15 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -703,7 +700,126 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colando o meu código teste que funcionou no Main
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -49,6 +49,9 @@
     <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
   </si>
   <si>
+    <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
+  </si>
+  <si>
     <t>1992 Gasolina</t>
   </si>
   <si>
@@ -85,6 +88,12 @@
     <t>2004 Diesel</t>
   </si>
   <si>
+    <t>2015 Diesel</t>
+  </si>
+  <si>
+    <t>2014 Diesel</t>
+  </si>
+  <si>
     <t>038003-2</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
     <t>060001-6</t>
   </si>
   <si>
+    <t>060003-2</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 11097.00</t>
   </si>
   <si>
@@ -152,6 +164,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 36756.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 108542.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102457.00</t>
   </si>
 </sst>
 </file>
@@ -509,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,13 +558,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -557,13 +575,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -574,13 +592,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -591,13 +609,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -608,13 +626,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -625,13 +643,13 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -642,13 +660,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -659,13 +677,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -676,13 +694,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -693,13 +711,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -710,13 +728,13 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -727,13 +745,13 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -744,13 +762,13 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -761,13 +779,13 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -778,13 +796,13 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -795,13 +813,13 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -812,13 +830,13 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -829,13 +847,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -846,13 +864,47 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testar maneira de não fazer pegar os modelos da marca anterior
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="239">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Agrale</t>
   </si>
   <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>AM Gen</t>
+  </si>
+  <si>
     <t>Integra GS 1.8</t>
   </si>
   <si>
@@ -52,6 +58,84 @@
     <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
   </si>
   <si>
+    <t>MARRUÁ AM 100 2.8 CD TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 150 2.8  CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 150 2.8 CD TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 2.8  CD TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 2.8 CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Esc. 3.8 TDI Die.Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Escolar 2.8 TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Escolar 3.8 TDI Die. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Microbus 2.8 TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CD TDI Die. Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CD TDI Diesel (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CS TDI Die. Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CS TDI Diesel (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 50 2.8 140cv TDI Diesel</t>
+  </si>
+  <si>
+    <t>Hummer Hard-Top 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
+    <t>Hummer Open-Top 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
+    <t>Hummer Wagon 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
+    <t>DB12 Coupe 4.0 V8 680cv</t>
+  </si>
+  <si>
+    <t>DB12 Volante 4.0 V8 680cv</t>
+  </si>
+  <si>
+    <t>DB9 Coupe 6.0 V12 510cv</t>
+  </si>
+  <si>
+    <t>DB9 Volante 6.0 V12 470cv</t>
+  </si>
+  <si>
+    <t>DBS Coupe 5.2 V12 725cv</t>
+  </si>
+  <si>
+    <t>DBX 4.0 V8 550cv</t>
+  </si>
+  <si>
+    <t>DBX707 4.0 V8 707cv</t>
+  </si>
+  <si>
+    <t>Rapide 6.0 V12 477cv</t>
+  </si>
+  <si>
+    <t>Rapide S 6.0 V12 550cv</t>
+  </si>
+  <si>
     <t>1992 Gasolina</t>
   </si>
   <si>
@@ -94,6 +178,78 @@
     <t>2014 Diesel</t>
   </si>
   <si>
+    <t>2013 Diesel</t>
+  </si>
+  <si>
+    <t>2012 Diesel</t>
+  </si>
+  <si>
+    <t>2011 Diesel</t>
+  </si>
+  <si>
+    <t>2010 Diesel</t>
+  </si>
+  <si>
+    <t>2009 Diesel</t>
+  </si>
+  <si>
+    <t>2008 Diesel</t>
+  </si>
+  <si>
+    <t>2022 Diesel</t>
+  </si>
+  <si>
+    <t>2021 Diesel</t>
+  </si>
+  <si>
+    <t>2020 Diesel</t>
+  </si>
+  <si>
+    <t>2019 Diesel</t>
+  </si>
+  <si>
+    <t>2018 Diesel</t>
+  </si>
+  <si>
+    <t>2017 Diesel</t>
+  </si>
+  <si>
+    <t>2016 Diesel</t>
+  </si>
+  <si>
+    <t>Zero KM Diesel</t>
+  </si>
+  <si>
+    <t>2025 Diesel</t>
+  </si>
+  <si>
+    <t>2024 Diesel</t>
+  </si>
+  <si>
+    <t>2023 Diesel</t>
+  </si>
+  <si>
+    <t>2000 Diesel</t>
+  </si>
+  <si>
+    <t>1999 Diesel</t>
+  </si>
+  <si>
+    <t>1998 Diesel</t>
+  </si>
+  <si>
+    <t>1999 Gasolina</t>
+  </si>
+  <si>
+    <t>Zero KM Gasolina</t>
+  </si>
+  <si>
+    <t>2025 Gasolina</t>
+  </si>
+  <si>
+    <t>2024 Gasolina</t>
+  </si>
+  <si>
     <t>038003-2</t>
   </si>
   <si>
@@ -109,6 +265,69 @@
     <t>060003-2</t>
   </si>
   <si>
+    <t>060004-0</t>
+  </si>
+  <si>
+    <t>060005-9</t>
+  </si>
+  <si>
+    <t>060006-7</t>
+  </si>
+  <si>
+    <t>060008-3</t>
+  </si>
+  <si>
+    <t>060007-5</t>
+  </si>
+  <si>
+    <t>060014-8</t>
+  </si>
+  <si>
+    <t>060010-5</t>
+  </si>
+  <si>
+    <t>060011-3</t>
+  </si>
+  <si>
+    <t>060009-1</t>
+  </si>
+  <si>
+    <t>060013-0</t>
+  </si>
+  <si>
+    <t>060012-1</t>
+  </si>
+  <si>
+    <t>060016-4</t>
+  </si>
+  <si>
+    <t>060015-6</t>
+  </si>
+  <si>
+    <t>060002-4</t>
+  </si>
+  <si>
+    <t>037001-0</t>
+  </si>
+  <si>
+    <t>006009-7</t>
+  </si>
+  <si>
+    <t>006001-1</t>
+  </si>
+  <si>
+    <t>006002-0</t>
+  </si>
+  <si>
+    <t>085018-7</t>
+  </si>
+  <si>
+    <t>037002-9</t>
+  </si>
+  <si>
+    <t>037003-7</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 11097.00</t>
   </si>
   <si>
@@ -170,6 +389,348 @@
   </si>
   <si>
     <t xml:space="preserve"> 102457.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 94808.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92495.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 77133.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 64732.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50855.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45520.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 118402.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109313.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 105835.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 98655.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 79141.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67803.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56957.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52227.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49774.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109984.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102929.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95786.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90235.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 76651.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 61576.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52512.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 47788.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 123530.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 116892.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 110141.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 107454.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87847.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 69207.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60165.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57040.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 342477.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 323094.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 309449.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 232839.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 196563.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 151051.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 130818.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 127345.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 119707.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109489.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102295.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89100.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71438.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66077.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62211.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 319147.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 295759.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 272470.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 218838.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 182819.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 143191.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 128066.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 117176.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 107701.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99063.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92339.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 85809.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65829.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57637.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54453.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49790.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 871250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 720239.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 668533.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 625747.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 395995.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 370657.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 767261.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 673977.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 647026.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 593239.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 393070.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 367151.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 690496.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 568060.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 518150.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 484471.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 621203.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 516464.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 477859.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 446883.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 639491.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 531677.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 489059.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 456781.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 573663.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 462508.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 434991.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 406281.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 72391.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65190.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 55471.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 51567.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 426859.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21558.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14581.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21581.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17680.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17248.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13550.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29872.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29143.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23404.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22833.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3600000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 384365.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 332825.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 396648.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 351603.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 294624.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 453297.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 401677.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 348246.00</t>
   </si>
 </sst>
 </file>
@@ -527,7 +1088,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -555,16 +1116,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -572,16 +1133,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -589,16 +1150,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -606,16 +1167,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -623,16 +1184,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -640,16 +1201,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -657,16 +1218,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -674,16 +1235,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -691,16 +1252,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -708,16 +1269,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -725,16 +1286,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -742,16 +1303,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -759,16 +1320,16 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -776,16 +1337,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -793,16 +1354,16 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -810,16 +1371,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -827,16 +1388,16 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -844,16 +1405,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -861,16 +1422,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -878,16 +1439,16 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -895,16 +1456,2243 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D69" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>53</v>
+      </c>
+      <c r="D77" t="s">
+        <v>87</v>
+      </c>
+      <c r="E77" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>54</v>
+      </c>
+      <c r="D78" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
+        <v>55</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" t="s">
+        <v>87</v>
+      </c>
+      <c r="E80" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D82" t="s">
+        <v>87</v>
+      </c>
+      <c r="E82" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>59</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" t="s">
+        <v>87</v>
+      </c>
+      <c r="E84" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" t="s">
+        <v>88</v>
+      </c>
+      <c r="E85" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" t="s">
+        <v>68</v>
+      </c>
+      <c r="D86" t="s">
+        <v>88</v>
+      </c>
+      <c r="E86" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D87" t="s">
+        <v>88</v>
+      </c>
+      <c r="E87" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" t="s">
+        <v>88</v>
+      </c>
+      <c r="E88" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" t="s">
+        <v>89</v>
+      </c>
+      <c r="E89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>61</v>
+      </c>
+      <c r="D90" t="s">
+        <v>89</v>
+      </c>
+      <c r="E90" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" t="s">
+        <v>90</v>
+      </c>
+      <c r="E91" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D92" t="s">
+        <v>90</v>
+      </c>
+      <c r="E92" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" t="s">
+        <v>69</v>
+      </c>
+      <c r="D93" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D94" t="s">
+        <v>90</v>
+      </c>
+      <c r="E94" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" t="s">
+        <v>67</v>
+      </c>
+      <c r="D97" t="s">
+        <v>92</v>
+      </c>
+      <c r="E97" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" t="s">
+        <v>68</v>
+      </c>
+      <c r="D98" t="s">
+        <v>92</v>
+      </c>
+      <c r="E98" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99" t="s">
+        <v>92</v>
+      </c>
+      <c r="E99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100" t="s">
+        <v>92</v>
+      </c>
+      <c r="E100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" t="s">
+        <v>67</v>
+      </c>
+      <c r="D101" t="s">
+        <v>93</v>
+      </c>
+      <c r="E101" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" t="s">
+        <v>68</v>
+      </c>
+      <c r="D102" t="s">
+        <v>93</v>
+      </c>
+      <c r="E102" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103" t="s">
+        <v>93</v>
+      </c>
+      <c r="E103" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104" t="s">
+        <v>93</v>
+      </c>
+      <c r="E104" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" t="s">
         <v>25</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C105" t="s">
+        <v>67</v>
+      </c>
+      <c r="D105" t="s">
+        <v>94</v>
+      </c>
+      <c r="E105" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D106" t="s">
+        <v>94</v>
+      </c>
+      <c r="E106" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" t="s">
+        <v>69</v>
+      </c>
+      <c r="D107" t="s">
+        <v>94</v>
+      </c>
+      <c r="E107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" t="s">
+        <v>25</v>
+      </c>
+      <c r="C108" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108" t="s">
+        <v>94</v>
+      </c>
+      <c r="E108" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" t="s">
+        <v>26</v>
+      </c>
+      <c r="C109" t="s">
+        <v>67</v>
+      </c>
+      <c r="D109" t="s">
+        <v>95</v>
+      </c>
+      <c r="E109" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" t="s">
+        <v>68</v>
+      </c>
+      <c r="D110" t="s">
+        <v>95</v>
+      </c>
+      <c r="E110" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" t="s">
+        <v>95</v>
+      </c>
+      <c r="E111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" t="s">
+        <v>70</v>
+      </c>
+      <c r="D112" t="s">
+        <v>95</v>
+      </c>
+      <c r="E112" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" t="s">
+        <v>27</v>
+      </c>
+      <c r="C113" t="s">
+        <v>56</v>
+      </c>
+      <c r="D113" t="s">
+        <v>96</v>
+      </c>
+      <c r="E113" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>57</v>
+      </c>
+      <c r="D114" t="s">
+        <v>96</v>
+      </c>
+      <c r="E114" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" t="s">
+        <v>58</v>
+      </c>
+      <c r="D115" t="s">
+        <v>96</v>
+      </c>
+      <c r="E115" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" t="s">
+        <v>59</v>
+      </c>
+      <c r="D116" t="s">
+        <v>96</v>
+      </c>
+      <c r="E116" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" t="s">
+        <v>71</v>
+      </c>
+      <c r="D117" t="s">
+        <v>97</v>
+      </c>
+      <c r="E117" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118" t="s">
+        <v>72</v>
+      </c>
+      <c r="D118" t="s">
+        <v>98</v>
+      </c>
+      <c r="E118" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" t="s">
+        <v>73</v>
+      </c>
+      <c r="D119" t="s">
+        <v>98</v>
+      </c>
+      <c r="E119" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>29</v>
+      </c>
+      <c r="C120" t="s">
+        <v>42</v>
+      </c>
+      <c r="D120" t="s">
+        <v>99</v>
+      </c>
+      <c r="E120" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" t="s">
+        <v>43</v>
+      </c>
+      <c r="D121" t="s">
+        <v>99</v>
+      </c>
+      <c r="E121" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" t="s">
+        <v>44</v>
+      </c>
+      <c r="D122" t="s">
+        <v>99</v>
+      </c>
+      <c r="E122" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>45</v>
+      </c>
+      <c r="D123" t="s">
+        <v>99</v>
+      </c>
+      <c r="E123" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" t="s">
         <v>30</v>
       </c>
-      <c r="E22" t="s">
-        <v>51</v>
+      <c r="C124" t="s">
+        <v>74</v>
+      </c>
+      <c r="D124" t="s">
+        <v>100</v>
+      </c>
+      <c r="E124" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" t="s">
+        <v>30</v>
+      </c>
+      <c r="C125" t="s">
+        <v>42</v>
+      </c>
+      <c r="D125" t="s">
+        <v>100</v>
+      </c>
+      <c r="E125" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" t="s">
+        <v>43</v>
+      </c>
+      <c r="D126" t="s">
+        <v>100</v>
+      </c>
+      <c r="E126" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" t="s">
+        <v>44</v>
+      </c>
+      <c r="D127" t="s">
+        <v>100</v>
+      </c>
+      <c r="E127" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" t="s">
+        <v>75</v>
+      </c>
+      <c r="D128" t="s">
+        <v>101</v>
+      </c>
+      <c r="E128" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" t="s">
+        <v>76</v>
+      </c>
+      <c r="D129" t="s">
+        <v>97</v>
+      </c>
+      <c r="E129" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" t="s">
+        <v>77</v>
+      </c>
+      <c r="D130" t="s">
+        <v>97</v>
+      </c>
+      <c r="E130" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" t="s">
+        <v>32</v>
+      </c>
+      <c r="C131" t="s">
+        <v>71</v>
+      </c>
+      <c r="D131" t="s">
+        <v>102</v>
+      </c>
+      <c r="E131" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" t="s">
+        <v>72</v>
+      </c>
+      <c r="D132" t="s">
+        <v>102</v>
+      </c>
+      <c r="E132" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" t="s">
+        <v>32</v>
+      </c>
+      <c r="C133" t="s">
+        <v>73</v>
+      </c>
+      <c r="D133" t="s">
+        <v>102</v>
+      </c>
+      <c r="E133" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" t="s">
+        <v>33</v>
+      </c>
+      <c r="C134" t="s">
+        <v>71</v>
+      </c>
+      <c r="D134" t="s">
+        <v>103</v>
+      </c>
+      <c r="E134" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" t="s">
+        <v>72</v>
+      </c>
+      <c r="D135" t="s">
+        <v>103</v>
+      </c>
+      <c r="E135" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" t="s">
+        <v>73</v>
+      </c>
+      <c r="D136" t="s">
+        <v>103</v>
+      </c>
+      <c r="E136" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137" t="s">
+        <v>34</v>
+      </c>
+      <c r="C137" t="s">
+        <v>71</v>
+      </c>
+      <c r="D137" t="s">
+        <v>103</v>
+      </c>
+      <c r="E137" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" t="s">
+        <v>34</v>
+      </c>
+      <c r="C138" t="s">
+        <v>72</v>
+      </c>
+      <c r="D138" t="s">
+        <v>103</v>
+      </c>
+      <c r="E138" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>8</v>
+      </c>
+      <c r="B139" t="s">
+        <v>34</v>
+      </c>
+      <c r="C139" t="s">
+        <v>73</v>
+      </c>
+      <c r="D139" t="s">
+        <v>103</v>
+      </c>
+      <c r="E139" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" t="s">
+        <v>71</v>
+      </c>
+      <c r="D140" t="s">
+        <v>103</v>
+      </c>
+      <c r="E140" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141" t="s">
+        <v>35</v>
+      </c>
+      <c r="C141" t="s">
+        <v>72</v>
+      </c>
+      <c r="D141" t="s">
+        <v>103</v>
+      </c>
+      <c r="E141" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" t="s">
+        <v>73</v>
+      </c>
+      <c r="D142" t="s">
+        <v>103</v>
+      </c>
+      <c r="E142" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>36</v>
+      </c>
+      <c r="C143" t="s">
+        <v>71</v>
+      </c>
+      <c r="D143" t="s">
+        <v>103</v>
+      </c>
+      <c r="E143" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" t="s">
+        <v>36</v>
+      </c>
+      <c r="C144" t="s">
+        <v>72</v>
+      </c>
+      <c r="D144" t="s">
+        <v>103</v>
+      </c>
+      <c r="E144" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>36</v>
+      </c>
+      <c r="C145" t="s">
+        <v>73</v>
+      </c>
+      <c r="D145" t="s">
+        <v>103</v>
+      </c>
+      <c r="E145" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" t="s">
+        <v>71</v>
+      </c>
+      <c r="D146" t="s">
+        <v>103</v>
+      </c>
+      <c r="E146" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" t="s">
+        <v>37</v>
+      </c>
+      <c r="C147" t="s">
+        <v>72</v>
+      </c>
+      <c r="D147" t="s">
+        <v>103</v>
+      </c>
+      <c r="E147" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" t="s">
+        <v>37</v>
+      </c>
+      <c r="C148" t="s">
+        <v>73</v>
+      </c>
+      <c r="D148" t="s">
+        <v>103</v>
+      </c>
+      <c r="E148" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
+        <v>38</v>
+      </c>
+      <c r="C149" t="s">
+        <v>71</v>
+      </c>
+      <c r="D149" t="s">
+        <v>103</v>
+      </c>
+      <c r="E149" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" t="s">
+        <v>38</v>
+      </c>
+      <c r="C150" t="s">
+        <v>72</v>
+      </c>
+      <c r="D150" t="s">
+        <v>103</v>
+      </c>
+      <c r="E150" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" t="s">
+        <v>38</v>
+      </c>
+      <c r="C151" t="s">
+        <v>73</v>
+      </c>
+      <c r="D151" t="s">
+        <v>103</v>
+      </c>
+      <c r="E151" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" t="s">
+        <v>39</v>
+      </c>
+      <c r="C152" t="s">
+        <v>71</v>
+      </c>
+      <c r="D152" t="s">
+        <v>103</v>
+      </c>
+      <c r="E152" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" t="s">
+        <v>39</v>
+      </c>
+      <c r="C153" t="s">
+        <v>72</v>
+      </c>
+      <c r="D153" t="s">
+        <v>103</v>
+      </c>
+      <c r="E153" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Salvando - Para testar nova alteração que irei fazer
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="306">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Agrale</t>
   </si>
   <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>AM Gen</t>
+  </si>
+  <si>
     <t>Integra GS 1.8</t>
   </si>
   <si>
@@ -61,6 +67,96 @@
     <t>MARRUÁ AM 150 2.8 CD TDI Diesel</t>
   </si>
   <si>
+    <t>MARRUÁ AM 200 2.8  CD TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 2.8 CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Esc. 3.8 TDI Die.Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Escolar 2.8 TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Escolar 3.8 TDI Die. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 200 Microbus 2.8 TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CD TDI Die. Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CD TDI Diesel (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CS TDI Die. Aut. (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 250 3.8 CS TDI Diesel (E6)</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 50 2.8 140cv TDI Diesel</t>
+  </si>
+  <si>
+    <t>145 Elegant 1.7/1.8 16V</t>
+  </si>
+  <si>
+    <t>145 Elegant 2.0 16V</t>
+  </si>
+  <si>
+    <t>145 Quadrifoglio 2.0</t>
+  </si>
+  <si>
+    <t>145 QV</t>
+  </si>
+  <si>
+    <t>147 2.0 16V 148cv 4p Semi-Aut.</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>155 Super</t>
+  </si>
+  <si>
+    <t>156 2.5 V6 24V 190cv 4p Aut.</t>
+  </si>
+  <si>
+    <t>156 Sport Wagon 2.0 16V</t>
+  </si>
+  <si>
+    <t>156 Sport Wagon 2.5 V6 24V 4p Aut.</t>
+  </si>
+  <si>
+    <t>156 TS/Sport/Elegant 2.0 16V</t>
+  </si>
+  <si>
+    <t>164 3.0 V6</t>
+  </si>
+  <si>
+    <t>164 Super V6 24V</t>
+  </si>
+  <si>
+    <t>166 3.0 V6 24V</t>
+  </si>
+  <si>
+    <t>2300 TI/TI-4</t>
+  </si>
+  <si>
+    <t>Spider 2.0/3.0</t>
+  </si>
+  <si>
+    <t>Hummer Hard-Top 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
+    <t>Hummer Open-Top 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
+    <t>Hummer Wagon 6.5 4x4 Diesel TB</t>
+  </si>
+  <si>
     <t>1992 Gasolina</t>
   </si>
   <si>
@@ -121,6 +217,75 @@
     <t>2008 Diesel</t>
   </si>
   <si>
+    <t>2022 Diesel</t>
+  </si>
+  <si>
+    <t>2021 Diesel</t>
+  </si>
+  <si>
+    <t>2020 Diesel</t>
+  </si>
+  <si>
+    <t>2019 Diesel</t>
+  </si>
+  <si>
+    <t>2018 Diesel</t>
+  </si>
+  <si>
+    <t>2017 Diesel</t>
+  </si>
+  <si>
+    <t>2016 Diesel</t>
+  </si>
+  <si>
+    <t>Zero KM Diesel</t>
+  </si>
+  <si>
+    <t>2025 Diesel</t>
+  </si>
+  <si>
+    <t>2024 Diesel</t>
+  </si>
+  <si>
+    <t>2023 Diesel</t>
+  </si>
+  <si>
+    <t>1999 Gasolina</t>
+  </si>
+  <si>
+    <t>2005 Gasolina</t>
+  </si>
+  <si>
+    <t>2004 Gasolina</t>
+  </si>
+  <si>
+    <t>2003 Gasolina</t>
+  </si>
+  <si>
+    <t>2002 Gasolina</t>
+  </si>
+  <si>
+    <t>2001 Gasolina</t>
+  </si>
+  <si>
+    <t>2000 Gasolina</t>
+  </si>
+  <si>
+    <t>1986 Gasolina</t>
+  </si>
+  <si>
+    <t>1985 Gasolina</t>
+  </si>
+  <si>
+    <t>2000 Diesel</t>
+  </si>
+  <si>
+    <t>1999 Diesel</t>
+  </si>
+  <si>
+    <t>1998 Diesel</t>
+  </si>
+  <si>
     <t>038003-2</t>
   </si>
   <si>
@@ -145,6 +310,96 @@
     <t>060006-7</t>
   </si>
   <si>
+    <t>060008-3</t>
+  </si>
+  <si>
+    <t>060007-5</t>
+  </si>
+  <si>
+    <t>060014-8</t>
+  </si>
+  <si>
+    <t>060010-5</t>
+  </si>
+  <si>
+    <t>060011-3</t>
+  </si>
+  <si>
+    <t>060009-1</t>
+  </si>
+  <si>
+    <t>060013-0</t>
+  </si>
+  <si>
+    <t>060012-1</t>
+  </si>
+  <si>
+    <t>060016-4</t>
+  </si>
+  <si>
+    <t>060015-6</t>
+  </si>
+  <si>
+    <t>060002-4</t>
+  </si>
+  <si>
+    <t>006009-7</t>
+  </si>
+  <si>
+    <t>006001-1</t>
+  </si>
+  <si>
+    <t>006002-0</t>
+  </si>
+  <si>
+    <t>006008-9</t>
+  </si>
+  <si>
+    <t>006017-8</t>
+  </si>
+  <si>
+    <t>006003-8</t>
+  </si>
+  <si>
+    <t>006004-6</t>
+  </si>
+  <si>
+    <t>006015-1</t>
+  </si>
+  <si>
+    <t>006014-3</t>
+  </si>
+  <si>
+    <t>006016-0</t>
+  </si>
+  <si>
+    <t>006010-0</t>
+  </si>
+  <si>
+    <t>006005-4</t>
+  </si>
+  <si>
+    <t>006006-2</t>
+  </si>
+  <si>
+    <t>006011-9</t>
+  </si>
+  <si>
+    <t>006013-5</t>
+  </si>
+  <si>
+    <t>006007-0</t>
+  </si>
+  <si>
+    <t>037001-0</t>
+  </si>
+  <si>
+    <t>037002-9</t>
+  </si>
+  <si>
+    <t>037003-7</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 11097.00</t>
   </si>
   <si>
@@ -262,9 +517,6 @@
     <t xml:space="preserve"> 95786.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 90235.00</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 76651.00</t>
   </si>
   <si>
@@ -290,6 +542,396 @@
   </si>
   <si>
     <t xml:space="preserve"> 87847.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 69207.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60165.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57040.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 342477.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 323094.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 309449.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 232839.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 196563.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 151051.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 130818.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 127345.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 119707.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109489.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102295.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89100.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71438.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66077.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62211.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 319147.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 295759.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 272470.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 218838.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 182819.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 143191.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 128066.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 117176.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 107701.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99063.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92339.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 85809.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65829.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57637.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54453.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49790.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 871250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 720239.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 668533.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 625747.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 395995.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 370657.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 767261.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 673977.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 647026.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 593239.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 393070.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 367151.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 690496.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 568060.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 518150.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 484471.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 621203.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 516464.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 477859.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 446883.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 639491.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 531677.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 489059.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 456781.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 573663.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 462508.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 434991.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 406281.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 72391.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65190.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 55471.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 51567.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27313.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21558.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14581.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13265.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21581.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17680.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17248.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13550.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29872.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29143.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23404.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22833.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22449.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18647.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18192.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92142.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89894.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87701.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19511.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18466.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15931.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24925.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24317.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19754.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 104853.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32424.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49978.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45101.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 74355.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71998.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75561.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 70007.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 58514.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57086.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29151.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28440.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27102.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19575.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13455.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11701.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28869.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28164.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89797.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 86004.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 83906.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 81859.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71424.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8070.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7072.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133185.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 129936.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92099.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41220.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32289.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27713.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 426859.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 384365.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 332825.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 396648.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 351603.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 294624.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 453297.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 401677.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 348246.00</t>
   </si>
 </sst>
 </file>
@@ -647,7 +1289,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -675,16 +1317,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -692,16 +1334,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -709,16 +1351,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -726,16 +1368,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -743,16 +1385,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -760,16 +1402,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -777,16 +1419,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -794,16 +1436,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -811,16 +1453,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -828,16 +1470,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -845,16 +1487,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -862,16 +1504,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -879,16 +1521,16 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -896,16 +1538,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -913,16 +1555,16 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -930,16 +1572,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -947,16 +1589,16 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -964,16 +1606,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -981,16 +1623,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -998,16 +1640,16 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1015,16 +1657,16 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1032,16 +1674,16 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1049,16 +1691,16 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1066,16 +1708,16 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1083,16 +1725,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1100,16 +1742,16 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1117,16 +1759,16 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1134,16 +1776,16 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1151,16 +1793,16 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1168,16 +1810,16 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1185,16 +1827,16 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1202,16 +1844,16 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1219,16 +1861,16 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1236,16 +1878,16 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1253,16 +1895,16 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1270,16 +1912,16 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1287,16 +1929,16 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1304,16 +1946,16 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1321,16 +1963,16 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1338,16 +1980,16 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1355,16 +1997,16 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1372,16 +2014,16 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1389,16 +2031,16 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1406,16 +2048,16 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1423,16 +2065,16 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E46" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1440,16 +2082,16 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1457,16 +2099,16 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1474,16 +2116,16 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1491,16 +2133,2226 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" t="s">
+        <v>98</v>
+      </c>
+      <c r="E60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" t="s">
+        <v>98</v>
+      </c>
+      <c r="E62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" t="s">
+        <v>98</v>
+      </c>
+      <c r="E65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66" t="s">
+        <v>98</v>
+      </c>
+      <c r="E66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E67" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" t="s">
+        <v>99</v>
+      </c>
+      <c r="E69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" t="s">
+        <v>99</v>
+      </c>
+      <c r="E71" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" t="s">
+        <v>99</v>
+      </c>
+      <c r="E73" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>99</v>
+      </c>
+      <c r="E76" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>99</v>
+      </c>
+      <c r="E77" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>99</v>
+      </c>
+      <c r="E78" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" t="s">
+        <v>99</v>
+      </c>
+      <c r="E79" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>63</v>
+      </c>
+      <c r="D80" t="s">
+        <v>99</v>
+      </c>
+      <c r="E80" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" t="s">
+        <v>99</v>
+      </c>
+      <c r="E81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" t="s">
+        <v>99</v>
+      </c>
+      <c r="E82" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" t="s">
+        <v>99</v>
+      </c>
+      <c r="E83" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>55</v>
+      </c>
+      <c r="D84" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D86" t="s">
+        <v>100</v>
+      </c>
+      <c r="E86" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" t="s">
+        <v>76</v>
+      </c>
+      <c r="D87" t="s">
+        <v>100</v>
+      </c>
+      <c r="E87" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" t="s">
+        <v>77</v>
+      </c>
+      <c r="D88" t="s">
+        <v>100</v>
+      </c>
+      <c r="E88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>67</v>
+      </c>
+      <c r="D89" t="s">
+        <v>101</v>
+      </c>
+      <c r="E89" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>68</v>
+      </c>
+      <c r="D90" t="s">
+        <v>101</v>
+      </c>
+      <c r="E90" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
+      </c>
+      <c r="D91" t="s">
+        <v>102</v>
+      </c>
+      <c r="E91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>75</v>
+      </c>
+      <c r="D92" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s">
+        <v>102</v>
+      </c>
+      <c r="E93" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" t="s">
+        <v>77</v>
+      </c>
+      <c r="D94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E94" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>67</v>
+      </c>
+      <c r="D95" t="s">
+        <v>103</v>
+      </c>
+      <c r="E95" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>68</v>
+      </c>
+      <c r="D96" t="s">
+        <v>103</v>
+      </c>
+      <c r="E96" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97" t="s">
+        <v>104</v>
+      </c>
+      <c r="E97" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" t="s">
+        <v>75</v>
+      </c>
+      <c r="D98" t="s">
+        <v>104</v>
+      </c>
+      <c r="E98" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>76</v>
+      </c>
+      <c r="D99" t="s">
+        <v>104</v>
+      </c>
+      <c r="E99" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" t="s">
+        <v>77</v>
+      </c>
+      <c r="D100" t="s">
+        <v>104</v>
+      </c>
+      <c r="E100" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" t="s">
+        <v>74</v>
+      </c>
+      <c r="D101" t="s">
+        <v>105</v>
+      </c>
+      <c r="E101" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" t="s">
+        <v>75</v>
+      </c>
+      <c r="D102" t="s">
+        <v>105</v>
+      </c>
+      <c r="E102" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>76</v>
+      </c>
+      <c r="D103" t="s">
+        <v>105</v>
+      </c>
+      <c r="E103" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>77</v>
+      </c>
+      <c r="D104" t="s">
+        <v>105</v>
+      </c>
+      <c r="E104" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" t="s">
+        <v>25</v>
+      </c>
+      <c r="C105" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" t="s">
+        <v>106</v>
+      </c>
+      <c r="E105" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" t="s">
+        <v>106</v>
+      </c>
+      <c r="E106" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" t="s">
+        <v>76</v>
+      </c>
+      <c r="D107" t="s">
+        <v>106</v>
+      </c>
+      <c r="E107" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" t="s">
+        <v>25</v>
+      </c>
+      <c r="C108" t="s">
+        <v>77</v>
+      </c>
+      <c r="D108" t="s">
+        <v>106</v>
+      </c>
+      <c r="E108" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" t="s">
+        <v>26</v>
+      </c>
+      <c r="C109" t="s">
+        <v>74</v>
+      </c>
+      <c r="D109" t="s">
+        <v>107</v>
+      </c>
+      <c r="E109" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" t="s">
+        <v>75</v>
+      </c>
+      <c r="D110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" t="s">
+        <v>76</v>
+      </c>
+      <c r="D111" t="s">
+        <v>107</v>
+      </c>
+      <c r="E111" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" t="s">
+        <v>77</v>
+      </c>
+      <c r="D112" t="s">
+        <v>107</v>
+      </c>
+      <c r="E112" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" t="s">
+        <v>27</v>
+      </c>
+      <c r="C113" t="s">
+        <v>63</v>
+      </c>
+      <c r="D113" t="s">
+        <v>108</v>
+      </c>
+      <c r="E113" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>64</v>
+      </c>
+      <c r="D114" t="s">
+        <v>108</v>
+      </c>
+      <c r="E114" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" t="s">
+        <v>108</v>
+      </c>
+      <c r="E115" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" t="s">
+        <v>66</v>
+      </c>
+      <c r="D116" t="s">
+        <v>108</v>
+      </c>
+      <c r="E116" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" t="s">
+        <v>78</v>
+      </c>
+      <c r="D117" t="s">
+        <v>109</v>
+      </c>
+      <c r="E117" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118" t="s">
+        <v>49</v>
+      </c>
+      <c r="D118" t="s">
+        <v>109</v>
+      </c>
+      <c r="E118" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" t="s">
+        <v>50</v>
+      </c>
+      <c r="D119" t="s">
+        <v>109</v>
+      </c>
+      <c r="E119" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" t="s">
+        <v>51</v>
+      </c>
+      <c r="D120" t="s">
+        <v>109</v>
+      </c>
+      <c r="E120" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" t="s">
+        <v>49</v>
+      </c>
+      <c r="D121" t="s">
+        <v>110</v>
+      </c>
+      <c r="E121" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" t="s">
+        <v>50</v>
+      </c>
+      <c r="D122" t="s">
+        <v>110</v>
+      </c>
+      <c r="E122" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>51</v>
+      </c>
+      <c r="D123" t="s">
+        <v>110</v>
+      </c>
+      <c r="E123" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" t="s">
+        <v>29</v>
+      </c>
+      <c r="C124" t="s">
+        <v>52</v>
+      </c>
+      <c r="D124" t="s">
+        <v>110</v>
+      </c>
+      <c r="E124" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" t="s">
+        <v>30</v>
+      </c>
+      <c r="C125" t="s">
+        <v>78</v>
+      </c>
+      <c r="D125" t="s">
+        <v>111</v>
+      </c>
+      <c r="E125" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" t="s">
+        <v>49</v>
+      </c>
+      <c r="D126" t="s">
+        <v>111</v>
+      </c>
+      <c r="E126" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" t="s">
+        <v>50</v>
+      </c>
+      <c r="D127" t="s">
+        <v>111</v>
+      </c>
+      <c r="E127" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" t="s">
+        <v>51</v>
+      </c>
+      <c r="D128" t="s">
+        <v>111</v>
+      </c>
+      <c r="E128" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" t="s">
         <v>31</v>
       </c>
-      <c r="D50" t="s">
+      <c r="C129" t="s">
+        <v>49</v>
+      </c>
+      <c r="D129" t="s">
+        <v>112</v>
+      </c>
+      <c r="E129" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" t="s">
+        <v>50</v>
+      </c>
+      <c r="D130" t="s">
+        <v>112</v>
+      </c>
+      <c r="E130" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" t="s">
+        <v>51</v>
+      </c>
+      <c r="D131" t="s">
+        <v>112</v>
+      </c>
+      <c r="E131" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" t="s">
+        <v>79</v>
+      </c>
+      <c r="D132" t="s">
+        <v>113</v>
+      </c>
+      <c r="E132" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" t="s">
+        <v>32</v>
+      </c>
+      <c r="C133" t="s">
+        <v>80</v>
+      </c>
+      <c r="D133" t="s">
+        <v>113</v>
+      </c>
+      <c r="E133" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" t="s">
+        <v>32</v>
+      </c>
+      <c r="C134" t="s">
+        <v>81</v>
+      </c>
+      <c r="D134" t="s">
+        <v>113</v>
+      </c>
+      <c r="E134" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D135" t="s">
+        <v>114</v>
+      </c>
+      <c r="E135" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" t="s">
+        <v>51</v>
+      </c>
+      <c r="D136" t="s">
+        <v>114</v>
+      </c>
+      <c r="E136" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" t="s">
+        <v>33</v>
+      </c>
+      <c r="C137" t="s">
+        <v>52</v>
+      </c>
+      <c r="D137" t="s">
+        <v>114</v>
+      </c>
+      <c r="E137" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B138" t="s">
+        <v>34</v>
+      </c>
+      <c r="C138" t="s">
+        <v>50</v>
+      </c>
+      <c r="D138" t="s">
+        <v>115</v>
+      </c>
+      <c r="E138" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>7</v>
+      </c>
+      <c r="B139" t="s">
+        <v>34</v>
+      </c>
+      <c r="C139" t="s">
+        <v>51</v>
+      </c>
+      <c r="D139" t="s">
+        <v>115</v>
+      </c>
+      <c r="E139" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>7</v>
+      </c>
+      <c r="B140" t="s">
+        <v>34</v>
+      </c>
+      <c r="C140" t="s">
+        <v>52</v>
+      </c>
+      <c r="D140" t="s">
+        <v>115</v>
+      </c>
+      <c r="E140" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>7</v>
+      </c>
+      <c r="B141" t="s">
+        <v>35</v>
+      </c>
+      <c r="C141" t="s">
+        <v>81</v>
+      </c>
+      <c r="D141" t="s">
+        <v>116</v>
+      </c>
+      <c r="E141" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>7</v>
+      </c>
+      <c r="B142" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" t="s">
+        <v>78</v>
+      </c>
+      <c r="D142" t="s">
+        <v>116</v>
+      </c>
+      <c r="E142" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143" t="s">
+        <v>36</v>
+      </c>
+      <c r="C143" t="s">
+        <v>82</v>
+      </c>
+      <c r="D143" t="s">
+        <v>117</v>
+      </c>
+      <c r="E143" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144" t="s">
+        <v>36</v>
+      </c>
+      <c r="C144" t="s">
+        <v>83</v>
+      </c>
+      <c r="D144" t="s">
+        <v>117</v>
+      </c>
+      <c r="E144" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145" t="s">
+        <v>80</v>
+      </c>
+      <c r="D145" t="s">
+        <v>118</v>
+      </c>
+      <c r="E145" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" t="s">
+        <v>81</v>
+      </c>
+      <c r="D146" t="s">
+        <v>118</v>
+      </c>
+      <c r="E146" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>7</v>
+      </c>
+      <c r="B147" t="s">
+        <v>38</v>
+      </c>
+      <c r="C147" t="s">
+        <v>82</v>
+      </c>
+      <c r="D147" t="s">
+        <v>119</v>
+      </c>
+      <c r="E147" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>7</v>
+      </c>
+      <c r="B148" t="s">
+        <v>38</v>
+      </c>
+      <c r="C148" t="s">
+        <v>83</v>
+      </c>
+      <c r="D148" t="s">
+        <v>119</v>
+      </c>
+      <c r="E148" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>7</v>
+      </c>
+      <c r="B149" t="s">
+        <v>38</v>
+      </c>
+      <c r="C149" t="s">
+        <v>84</v>
+      </c>
+      <c r="D149" t="s">
+        <v>119</v>
+      </c>
+      <c r="E149" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>7</v>
+      </c>
+      <c r="B150" t="s">
+        <v>38</v>
+      </c>
+      <c r="C150" t="s">
+        <v>78</v>
+      </c>
+      <c r="D150" t="s">
+        <v>119</v>
+      </c>
+      <c r="E150" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>7</v>
+      </c>
+      <c r="B151" t="s">
+        <v>39</v>
+      </c>
+      <c r="C151" t="s">
+        <v>51</v>
+      </c>
+      <c r="D151" t="s">
+        <v>120</v>
+      </c>
+      <c r="E151" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>7</v>
+      </c>
+      <c r="B152" t="s">
+        <v>39</v>
+      </c>
+      <c r="C152" t="s">
+        <v>52</v>
+      </c>
+      <c r="D152" t="s">
+        <v>120</v>
+      </c>
+      <c r="E152" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153" t="s">
+        <v>39</v>
+      </c>
+      <c r="C153" t="s">
+        <v>53</v>
+      </c>
+      <c r="D153" t="s">
+        <v>120</v>
+      </c>
+      <c r="E153" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>7</v>
+      </c>
+      <c r="B154" t="s">
+        <v>39</v>
+      </c>
+      <c r="C154" t="s">
+        <v>54</v>
+      </c>
+      <c r="D154" t="s">
+        <v>120</v>
+      </c>
+      <c r="E154" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>7</v>
+      </c>
+      <c r="B155" t="s">
+        <v>39</v>
+      </c>
+      <c r="C155" t="s">
+        <v>47</v>
+      </c>
+      <c r="D155" t="s">
+        <v>120</v>
+      </c>
+      <c r="E155" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156" t="s">
+        <v>39</v>
+      </c>
+      <c r="C156" t="s">
+        <v>48</v>
+      </c>
+      <c r="D156" t="s">
+        <v>120</v>
+      </c>
+      <c r="E156" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" t="s">
+        <v>40</v>
+      </c>
+      <c r="C157" t="s">
+        <v>51</v>
+      </c>
+      <c r="D157" t="s">
+        <v>121</v>
+      </c>
+      <c r="E157" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158" t="s">
+        <v>40</v>
+      </c>
+      <c r="C158" t="s">
+        <v>52</v>
+      </c>
+      <c r="D158" t="s">
+        <v>121</v>
+      </c>
+      <c r="E158" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" t="s">
+        <v>41</v>
+      </c>
+      <c r="C159" t="s">
+        <v>81</v>
+      </c>
+      <c r="D159" t="s">
+        <v>122</v>
+      </c>
+      <c r="E159" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>7</v>
+      </c>
+      <c r="B160" t="s">
+        <v>41</v>
+      </c>
+      <c r="C160" t="s">
+        <v>82</v>
+      </c>
+      <c r="D160" t="s">
+        <v>122</v>
+      </c>
+      <c r="E160" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" t="s">
+        <v>41</v>
+      </c>
+      <c r="C161" t="s">
+        <v>83</v>
+      </c>
+      <c r="D161" t="s">
+        <v>122</v>
+      </c>
+      <c r="E161" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>7</v>
+      </c>
+      <c r="B162" t="s">
+        <v>41</v>
+      </c>
+      <c r="C162" t="s">
+        <v>84</v>
+      </c>
+      <c r="D162" t="s">
+        <v>122</v>
+      </c>
+      <c r="E162" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>41</v>
+      </c>
+      <c r="C163" t="s">
+        <v>78</v>
+      </c>
+      <c r="D163" t="s">
+        <v>122</v>
+      </c>
+      <c r="E163" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>7</v>
+      </c>
+      <c r="B164" t="s">
         <v>42</v>
       </c>
-      <c r="E50" t="s">
-        <v>91</v>
+      <c r="C164" t="s">
+        <v>85</v>
+      </c>
+      <c r="D164" t="s">
+        <v>123</v>
+      </c>
+      <c r="E164" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165" t="s">
+        <v>42</v>
+      </c>
+      <c r="C165" t="s">
+        <v>86</v>
+      </c>
+      <c r="D165" t="s">
+        <v>123</v>
+      </c>
+      <c r="E165" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" t="s">
+        <v>43</v>
+      </c>
+      <c r="C166" t="s">
+        <v>50</v>
+      </c>
+      <c r="D166" t="s">
+        <v>124</v>
+      </c>
+      <c r="E166" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" t="s">
+        <v>43</v>
+      </c>
+      <c r="C167" t="s">
+        <v>51</v>
+      </c>
+      <c r="D167" t="s">
+        <v>124</v>
+      </c>
+      <c r="E167" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168" t="s">
+        <v>52</v>
+      </c>
+      <c r="D168" t="s">
+        <v>124</v>
+      </c>
+      <c r="E168" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" t="s">
+        <v>54</v>
+      </c>
+      <c r="D169" t="s">
+        <v>124</v>
+      </c>
+      <c r="E169" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" t="s">
+        <v>43</v>
+      </c>
+      <c r="C170" t="s">
+        <v>47</v>
+      </c>
+      <c r="D170" t="s">
+        <v>124</v>
+      </c>
+      <c r="E170" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>43</v>
+      </c>
+      <c r="C171" t="s">
+        <v>48</v>
+      </c>
+      <c r="D171" t="s">
+        <v>124</v>
+      </c>
+      <c r="E171" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" t="s">
+        <v>44</v>
+      </c>
+      <c r="C172" t="s">
+        <v>87</v>
+      </c>
+      <c r="D172" t="s">
+        <v>125</v>
+      </c>
+      <c r="E172" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" t="s">
+        <v>44</v>
+      </c>
+      <c r="C173" t="s">
+        <v>88</v>
+      </c>
+      <c r="D173" t="s">
+        <v>125</v>
+      </c>
+      <c r="E173" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174" t="s">
+        <v>44</v>
+      </c>
+      <c r="C174" t="s">
+        <v>89</v>
+      </c>
+      <c r="D174" t="s">
+        <v>125</v>
+      </c>
+      <c r="E174" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" t="s">
+        <v>45</v>
+      </c>
+      <c r="C175" t="s">
+        <v>87</v>
+      </c>
+      <c r="D175" t="s">
+        <v>126</v>
+      </c>
+      <c r="E175" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176" t="s">
+        <v>45</v>
+      </c>
+      <c r="C176" t="s">
+        <v>88</v>
+      </c>
+      <c r="D176" t="s">
+        <v>126</v>
+      </c>
+      <c r="E176" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177" t="s">
+        <v>45</v>
+      </c>
+      <c r="C177" t="s">
+        <v>89</v>
+      </c>
+      <c r="D177" t="s">
+        <v>126</v>
+      </c>
+      <c r="E177" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178" t="s">
+        <v>46</v>
+      </c>
+      <c r="C178" t="s">
+        <v>87</v>
+      </c>
+      <c r="D178" t="s">
+        <v>127</v>
+      </c>
+      <c r="E178" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>8</v>
+      </c>
+      <c r="B179" t="s">
+        <v>46</v>
+      </c>
+      <c r="C179" t="s">
+        <v>88</v>
+      </c>
+      <c r="D179" t="s">
+        <v>127</v>
+      </c>
+      <c r="E179" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>8</v>
+      </c>
+      <c r="B180" t="s">
+        <v>46</v>
+      </c>
+      <c r="C180" t="s">
+        <v>89</v>
+      </c>
+      <c r="D180" t="s">
+        <v>127</v>
+      </c>
+      <c r="E180" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Passando para o principal/MAIN
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="87">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -34,19 +34,244 @@
     <t>Mes Referencia</t>
   </si>
   <si>
-    <t>AM Gen</t>
-  </si>
-  <si>
-    <t>Hummer Hard-Top 6.5 4x4 Diesel TB</t>
-  </si>
-  <si>
-    <t>2000 Diesel</t>
-  </si>
-  <si>
-    <t>037001-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 426859.00</t>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>Agrale</t>
+  </si>
+  <si>
+    <t>Integra GS 1.8</t>
+  </si>
+  <si>
+    <t>Legend 3.2/3.5</t>
+  </si>
+  <si>
+    <t>NSX 3.0</t>
+  </si>
+  <si>
+    <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 100 2.8 CD TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 150 2.8  CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>1992 Gasolina</t>
+  </si>
+  <si>
+    <t>1991 Gasolina</t>
+  </si>
+  <si>
+    <t>1998 Gasolina</t>
+  </si>
+  <si>
+    <t>1997 Gasolina</t>
+  </si>
+  <si>
+    <t>1996 Gasolina</t>
+  </si>
+  <si>
+    <t>1995 Gasolina</t>
+  </si>
+  <si>
+    <t>1994 Gasolina</t>
+  </si>
+  <si>
+    <t>1993 Gasolina</t>
+  </si>
+  <si>
+    <t>2007 Diesel</t>
+  </si>
+  <si>
+    <t>2006 Diesel</t>
+  </si>
+  <si>
+    <t>2005 Diesel</t>
+  </si>
+  <si>
+    <t>2004 Diesel</t>
+  </si>
+  <si>
+    <t>2015 Diesel</t>
+  </si>
+  <si>
+    <t>2014 Diesel</t>
+  </si>
+  <si>
+    <t>2013 Diesel</t>
+  </si>
+  <si>
+    <t>2012 Diesel</t>
+  </si>
+  <si>
+    <t>2011 Diesel</t>
+  </si>
+  <si>
+    <t>2010 Diesel</t>
+  </si>
+  <si>
+    <t>2009 Diesel</t>
+  </si>
+  <si>
+    <t>2008 Diesel</t>
+  </si>
+  <si>
+    <t>038003-2</t>
+  </si>
+  <si>
+    <t>038002-4</t>
+  </si>
+  <si>
+    <t>038001-6</t>
+  </si>
+  <si>
+    <t>060001-6</t>
+  </si>
+  <si>
+    <t>060003-2</t>
+  </si>
+  <si>
+    <t>060004-0</t>
+  </si>
+  <si>
+    <t>060005-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11097.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10366.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25397.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22580.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21233.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19084.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18267.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16282.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14802.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14219.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40991.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39550.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38236.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36538.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33397.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 48251.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44511.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43362.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36756.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 108542.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102457.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 94808.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92495.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 77133.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 64732.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50855.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45520.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 118402.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109313.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 105835.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 98655.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 79141.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67803.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56957.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52227.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49774.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 109984.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 102929.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95786.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90235.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 76651.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 61576.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52512.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 47788.00</t>
   </si>
   <si>
     <t>junho de 2025</t>
@@ -407,7 +632,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,19 +663,879 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adaptando para caminhões e motos
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="333">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -181,6 +181,30 @@
     <t>DBX707 4.0 V8 707cv</t>
   </si>
   <si>
+    <t>Rapide 6.0 V12 477cv</t>
+  </si>
+  <si>
+    <t>Rapide S 6.0 V12 550cv</t>
+  </si>
+  <si>
+    <t>Vanquish V12 6.0 565cv</t>
+  </si>
+  <si>
+    <t>Vantage 6.0 V12 510cv</t>
+  </si>
+  <si>
+    <t>Vantage Coupe 4.7 V8 425cv</t>
+  </si>
+  <si>
+    <t>Vantage Cupê  4.0 V8 510cv</t>
+  </si>
+  <si>
+    <t>Vantage Cupê F1 Edition 4.0 V8 535cv</t>
+  </si>
+  <si>
+    <t>Vantage Roadster 4.7 V8 420cv</t>
+  </si>
+  <si>
     <t>1999 Gasolina</t>
   </si>
   <si>
@@ -280,6 +304,12 @@
     <t>2022 Gasolina</t>
   </si>
   <si>
+    <t>2012 Gasolina</t>
+  </si>
+  <si>
+    <t>2010 Gasolina</t>
+  </si>
+  <si>
     <t>006009-7</t>
   </si>
   <si>
@@ -415,6 +445,30 @@
     <t>085016-0</t>
   </si>
   <si>
+    <t>085007-1</t>
+  </si>
+  <si>
+    <t>085009-8</t>
+  </si>
+  <si>
+    <t>085010-1</t>
+  </si>
+  <si>
+    <t>085004-7</t>
+  </si>
+  <si>
+    <t>085002-0</t>
+  </si>
+  <si>
+    <t>085012-8</t>
+  </si>
+  <si>
+    <t>085013-6</t>
+  </si>
+  <si>
+    <t>085003-9</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 27313.00</t>
   </si>
   <si>
@@ -899,6 +953,63 @@
   </si>
   <si>
     <t xml:space="preserve"> 2502679.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 694217.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 607011.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1296696.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1032188.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1784133.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1616174.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 476063.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 638283.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 591028.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 528207.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 515323.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2800750.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2200329.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1739268.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1647750.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1770690.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1706250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 588516.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 521625.00</t>
   </si>
   <si>
     <t>junho de 2025</t>
@@ -1259,7 +1370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1293,16 +1404,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1313,16 +1424,16 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1333,16 +1444,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1353,16 +1464,16 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1373,16 +1484,16 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="F6" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1393,16 +1504,16 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1413,16 +1524,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1433,16 +1544,16 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="F9" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1453,16 +1564,16 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1473,16 +1584,16 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1493,16 +1604,16 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1513,16 +1624,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="F13" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1533,16 +1644,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1553,16 +1664,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="F15" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1573,16 +1684,16 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="F16" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1593,16 +1704,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="F17" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1613,16 +1724,16 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="F18" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1633,16 +1744,16 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="F19" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1653,16 +1764,16 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F20" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1673,16 +1784,16 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F21" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1693,16 +1804,16 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1713,16 +1824,16 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1733,16 +1844,16 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="F24" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1753,16 +1864,16 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="F25" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1773,16 +1884,16 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="F26" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1793,16 +1904,16 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="F27" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1813,16 +1924,16 @@
         <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="F28" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1833,16 +1944,16 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E29" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="F29" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1853,16 +1964,16 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="F30" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1873,16 +1984,16 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="F31" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1893,16 +2004,16 @@
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="F32" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1913,16 +2024,16 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E33" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="F33" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1933,16 +2044,16 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E34" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="F34" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1953,16 +2064,16 @@
         <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="F35" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1973,16 +2084,16 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E36" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="F36" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1993,16 +2104,16 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="F37" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2013,16 +2124,16 @@
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="F38" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2033,16 +2144,16 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E39" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2053,16 +2164,16 @@
         <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E40" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="F40" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2073,16 +2184,16 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="F41" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2093,16 +2204,16 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="F42" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2113,16 +2224,16 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F43" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2133,16 +2244,16 @@
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="F44" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2153,16 +2264,16 @@
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E45" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F45" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2173,16 +2284,16 @@
         <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E46" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="F46" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2193,16 +2304,16 @@
         <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E47" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="F47" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2213,16 +2324,16 @@
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E48" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="F48" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2233,16 +2344,16 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E49" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="F49" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2253,16 +2364,16 @@
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E50" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="F50" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2273,16 +2384,16 @@
         <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E51" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="F51" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2293,16 +2404,16 @@
         <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E52" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2313,16 +2424,16 @@
         <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E53" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="F53" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2333,16 +2444,16 @@
         <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E54" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="F54" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2353,16 +2464,16 @@
         <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E55" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="F55" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2373,16 +2484,16 @@
         <v>25</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E56" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F56" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2393,16 +2504,16 @@
         <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D57" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E57" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="F57" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2413,16 +2524,16 @@
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E58" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="F58" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2433,16 +2544,16 @@
         <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E59" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="F59" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2453,16 +2564,16 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E60" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="F60" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2473,16 +2584,16 @@
         <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E61" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="F61" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2493,16 +2604,16 @@
         <v>27</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D62" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E62" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="F62" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2513,16 +2624,16 @@
         <v>28</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D63" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E63" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="F63" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2533,16 +2644,16 @@
         <v>28</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D64" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E64" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="F64" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2553,16 +2664,16 @@
         <v>28</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D65" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E65" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="F65" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2573,16 +2684,16 @@
         <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D66" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E66" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="F66" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2593,16 +2704,16 @@
         <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E67" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="F67" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2613,16 +2724,16 @@
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E68" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="F68" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2633,16 +2744,16 @@
         <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D69" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E69" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="F69" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2653,16 +2764,16 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E70" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F70" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2673,16 +2784,16 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E71" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F71" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2693,16 +2804,16 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D72" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E72" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="F72" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2713,16 +2824,16 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E73" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="F73" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2733,16 +2844,16 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D74" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E74" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="F74" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2753,16 +2864,16 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E75" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="F75" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2773,16 +2884,16 @@
         <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D76" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E76" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="F76" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2793,16 +2904,16 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E77" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="F77" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2813,16 +2924,16 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D78" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E78" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="F78" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2833,16 +2944,16 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D79" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E79" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="F79" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2853,16 +2964,16 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D80" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E80" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="F80" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2873,16 +2984,16 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D81" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E81" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="F81" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2893,16 +3004,16 @@
         <v>32</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D82" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E82" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="F82" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2913,16 +3024,16 @@
         <v>32</v>
       </c>
       <c r="C83" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D83" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E83" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F83" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2933,16 +3044,16 @@
         <v>32</v>
       </c>
       <c r="C84" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D84" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E84" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="F84" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2953,16 +3064,16 @@
         <v>32</v>
       </c>
       <c r="C85" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D85" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E85" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="F85" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2973,16 +3084,16 @@
         <v>32</v>
       </c>
       <c r="C86" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D86" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E86" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="F86" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2993,16 +3104,16 @@
         <v>32</v>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D87" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="F87" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3013,16 +3124,16 @@
         <v>33</v>
       </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D88" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="F88" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3033,16 +3144,16 @@
         <v>33</v>
       </c>
       <c r="C89" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D89" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E89" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="F89" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3053,16 +3164,16 @@
         <v>33</v>
       </c>
       <c r="C90" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D90" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E90" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="F90" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3073,16 +3184,16 @@
         <v>33</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D91" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E91" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="F91" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3093,16 +3204,16 @@
         <v>34</v>
       </c>
       <c r="C92" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D92" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E92" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F92" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3113,16 +3224,16 @@
         <v>34</v>
       </c>
       <c r="C93" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D93" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E93" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="F93" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3133,16 +3244,16 @@
         <v>35</v>
       </c>
       <c r="C94" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D94" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E94" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="F94" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3153,16 +3264,16 @@
         <v>35</v>
       </c>
       <c r="C95" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D95" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E95" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="F95" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3173,16 +3284,16 @@
         <v>35</v>
       </c>
       <c r="C96" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D96" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="F96" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3193,16 +3304,16 @@
         <v>36</v>
       </c>
       <c r="C97" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D97" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E97" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="F97" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3213,16 +3324,16 @@
         <v>36</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D98" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E98" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="F98" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3233,16 +3344,16 @@
         <v>36</v>
       </c>
       <c r="C99" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D99" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E99" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="F99" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3253,16 +3364,16 @@
         <v>37</v>
       </c>
       <c r="C100" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D100" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E100" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="F100" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3273,16 +3384,16 @@
         <v>35</v>
       </c>
       <c r="C101" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D101" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E101" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="F101" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3293,16 +3404,16 @@
         <v>37</v>
       </c>
       <c r="C102" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D102" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E102" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="F102" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3313,16 +3424,16 @@
         <v>37</v>
       </c>
       <c r="C103" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D103" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E103" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="F103" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3333,16 +3444,16 @@
         <v>38</v>
       </c>
       <c r="C104" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D104" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E104" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="F104" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3353,16 +3464,16 @@
         <v>38</v>
       </c>
       <c r="C105" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D105" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E105" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="F105" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3373,16 +3484,16 @@
         <v>38</v>
       </c>
       <c r="C106" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D106" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E106" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="F106" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3393,16 +3504,16 @@
         <v>38</v>
       </c>
       <c r="C107" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D107" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E107" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="F107" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3413,16 +3524,16 @@
         <v>39</v>
       </c>
       <c r="C108" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D108" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E108" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="F108" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3433,16 +3544,16 @@
         <v>39</v>
       </c>
       <c r="C109" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D109" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E109" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="F109" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3453,16 +3564,16 @@
         <v>39</v>
       </c>
       <c r="C110" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D110" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E110" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="F110" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3473,16 +3584,16 @@
         <v>39</v>
       </c>
       <c r="C111" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D111" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E111" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="F111" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3493,16 +3604,16 @@
         <v>39</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D112" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E112" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="F112" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3513,16 +3624,16 @@
         <v>39</v>
       </c>
       <c r="C113" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D113" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E113" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="F113" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3533,16 +3644,16 @@
         <v>40</v>
       </c>
       <c r="C114" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D114" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E114" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="F114" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3553,16 +3664,16 @@
         <v>40</v>
       </c>
       <c r="C115" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D115" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E115" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="F115" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3573,16 +3684,16 @@
         <v>40</v>
       </c>
       <c r="C116" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D116" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E116" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="F116" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3593,16 +3704,16 @@
         <v>40</v>
       </c>
       <c r="C117" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D117" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E117" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="F117" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3613,16 +3724,16 @@
         <v>40</v>
       </c>
       <c r="C118" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D118" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E118" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="F118" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3633,16 +3744,16 @@
         <v>40</v>
       </c>
       <c r="C119" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D119" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E119" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="F119" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3653,16 +3764,16 @@
         <v>41</v>
       </c>
       <c r="C120" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D120" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E120" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="F120" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3673,16 +3784,16 @@
         <v>41</v>
       </c>
       <c r="C121" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D121" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E121" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="F121" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3693,16 +3804,16 @@
         <v>41</v>
       </c>
       <c r="C122" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D122" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E122" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="F122" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3713,16 +3824,16 @@
         <v>42</v>
       </c>
       <c r="C123" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D123" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E123" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="F123" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3733,16 +3844,16 @@
         <v>42</v>
       </c>
       <c r="C124" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D124" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E124" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="F124" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3753,16 +3864,16 @@
         <v>42</v>
       </c>
       <c r="C125" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D125" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E125" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="F125" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3773,16 +3884,16 @@
         <v>43</v>
       </c>
       <c r="C126" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D126" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E126" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="F126" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3793,16 +3904,16 @@
         <v>43</v>
       </c>
       <c r="C127" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D127" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E127" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="F127" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3813,16 +3924,16 @@
         <v>43</v>
       </c>
       <c r="C128" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D128" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E128" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="F128" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3833,16 +3944,16 @@
         <v>43</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D129" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E129" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="F129" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3853,16 +3964,16 @@
         <v>43</v>
       </c>
       <c r="C130" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D130" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E130" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="F130" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3873,16 +3984,16 @@
         <v>44</v>
       </c>
       <c r="C131" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D131" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E131" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="F131" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3893,16 +4004,16 @@
         <v>44</v>
       </c>
       <c r="C132" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D132" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E132" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="F132" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3913,16 +4024,16 @@
         <v>44</v>
       </c>
       <c r="C133" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D133" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E133" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="F133" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3933,16 +4044,16 @@
         <v>45</v>
       </c>
       <c r="C134" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D134" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E134" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="F134" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3953,16 +4064,16 @@
         <v>45</v>
       </c>
       <c r="C135" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D135" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E135" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="F135" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3973,16 +4084,16 @@
         <v>45</v>
       </c>
       <c r="C136" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D136" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E136" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="F136" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3993,16 +4104,16 @@
         <v>45</v>
       </c>
       <c r="C137" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D137" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E137" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="F137" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4013,16 +4124,16 @@
         <v>45</v>
       </c>
       <c r="C138" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D138" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E138" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="F138" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -4033,16 +4144,16 @@
         <v>45</v>
       </c>
       <c r="C139" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D139" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E139" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="F139" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4053,16 +4164,16 @@
         <v>46</v>
       </c>
       <c r="C140" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D140" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E140" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="F140" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -4073,16 +4184,16 @@
         <v>46</v>
       </c>
       <c r="C141" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D141" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E141" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="F141" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4093,16 +4204,16 @@
         <v>46</v>
       </c>
       <c r="C142" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D142" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E142" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="F142" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4113,16 +4224,16 @@
         <v>47</v>
       </c>
       <c r="C143" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D143" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E143" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="F143" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4133,16 +4244,16 @@
         <v>47</v>
       </c>
       <c r="C144" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D144" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E144" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="F144" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4153,16 +4264,16 @@
         <v>47</v>
       </c>
       <c r="C145" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D145" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E145" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="F145" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4173,16 +4284,16 @@
         <v>47</v>
       </c>
       <c r="C146" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D146" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E146" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="F146" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4193,16 +4304,16 @@
         <v>47</v>
       </c>
       <c r="C147" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D147" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E147" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="F147" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4213,16 +4324,16 @@
         <v>47</v>
       </c>
       <c r="C148" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D148" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E148" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="F148" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4233,16 +4344,16 @@
         <v>48</v>
       </c>
       <c r="C149" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D149" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E149" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="F149" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4253,16 +4364,16 @@
         <v>48</v>
       </c>
       <c r="C150" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D150" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E150" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="F150" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -4273,16 +4384,16 @@
         <v>48</v>
       </c>
       <c r="C151" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D151" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E151" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="F151" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -4293,16 +4404,16 @@
         <v>49</v>
       </c>
       <c r="C152" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D152" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E152" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="F152" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4313,16 +4424,16 @@
         <v>49</v>
       </c>
       <c r="C153" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D153" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E153" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="F153" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4333,16 +4444,16 @@
         <v>50</v>
       </c>
       <c r="C154" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D154" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E154" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="F154" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4353,16 +4464,16 @@
         <v>50</v>
       </c>
       <c r="C155" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D155" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E155" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="F155" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4373,16 +4484,16 @@
         <v>51</v>
       </c>
       <c r="C156" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D156" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="E156" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="F156" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4393,16 +4504,16 @@
         <v>52</v>
       </c>
       <c r="C157" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D157" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E157" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="F157" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4413,16 +4524,16 @@
         <v>52</v>
       </c>
       <c r="C158" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D158" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E158" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="F158" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4433,16 +4544,16 @@
         <v>53</v>
       </c>
       <c r="C159" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D159" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E159" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="F159" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4453,16 +4564,16 @@
         <v>53</v>
       </c>
       <c r="C160" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D160" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E160" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="F160" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -4473,16 +4584,16 @@
         <v>54</v>
       </c>
       <c r="C161" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D161" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E161" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="F161" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4493,16 +4604,16 @@
         <v>54</v>
       </c>
       <c r="C162" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D162" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E162" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="F162" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4513,16 +4624,16 @@
         <v>54</v>
       </c>
       <c r="C163" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D163" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E163" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="F163" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4533,16 +4644,396 @@
         <v>54</v>
       </c>
       <c r="C164" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D164" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E164" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="F164" t="s">
-        <v>295</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>55</v>
+      </c>
+      <c r="C165" t="s">
+        <v>96</v>
+      </c>
+      <c r="D165" t="s">
+        <v>143</v>
+      </c>
+      <c r="E165" t="s">
+        <v>313</v>
+      </c>
+      <c r="F165" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="s">
+        <v>9</v>
+      </c>
+      <c r="B166" t="s">
+        <v>55</v>
+      </c>
+      <c r="C166" t="s">
+        <v>93</v>
+      </c>
+      <c r="D166" t="s">
+        <v>143</v>
+      </c>
+      <c r="E166" t="s">
+        <v>314</v>
+      </c>
+      <c r="F166" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" t="s">
+        <v>56</v>
+      </c>
+      <c r="C167" t="s">
+        <v>91</v>
+      </c>
+      <c r="D167" t="s">
+        <v>144</v>
+      </c>
+      <c r="E167" t="s">
+        <v>315</v>
+      </c>
+      <c r="F167" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" t="s">
+        <v>56</v>
+      </c>
+      <c r="C168" t="s">
+        <v>92</v>
+      </c>
+      <c r="D168" t="s">
+        <v>144</v>
+      </c>
+      <c r="E168" t="s">
+        <v>316</v>
+      </c>
+      <c r="F168" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" t="s">
+        <v>57</v>
+      </c>
+      <c r="C169" t="s">
+        <v>91</v>
+      </c>
+      <c r="D169" t="s">
+        <v>145</v>
+      </c>
+      <c r="E169" t="s">
+        <v>317</v>
+      </c>
+      <c r="F169" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" t="s">
+        <v>57</v>
+      </c>
+      <c r="C170" t="s">
+        <v>92</v>
+      </c>
+      <c r="D170" t="s">
+        <v>145</v>
+      </c>
+      <c r="E170" t="s">
+        <v>318</v>
+      </c>
+      <c r="F170" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
+        <v>9</v>
+      </c>
+      <c r="B171" t="s">
+        <v>58</v>
+      </c>
+      <c r="C171" t="s">
+        <v>96</v>
+      </c>
+      <c r="D171" t="s">
+        <v>146</v>
+      </c>
+      <c r="E171" t="s">
+        <v>319</v>
+      </c>
+      <c r="F171" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" t="s">
+        <v>59</v>
+      </c>
+      <c r="C172" t="s">
+        <v>91</v>
+      </c>
+      <c r="D172" t="s">
+        <v>147</v>
+      </c>
+      <c r="E172" t="s">
+        <v>320</v>
+      </c>
+      <c r="F172" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" t="s">
+        <v>59</v>
+      </c>
+      <c r="C173" t="s">
+        <v>92</v>
+      </c>
+      <c r="D173" t="s">
+        <v>147</v>
+      </c>
+      <c r="E173" t="s">
+        <v>321</v>
+      </c>
+      <c r="F173" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" t="s">
+        <v>9</v>
+      </c>
+      <c r="B174" t="s">
+        <v>59</v>
+      </c>
+      <c r="C174" t="s">
+        <v>96</v>
+      </c>
+      <c r="D174" t="s">
+        <v>147</v>
+      </c>
+      <c r="E174" t="s">
+        <v>322</v>
+      </c>
+      <c r="F174" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" t="s">
+        <v>9</v>
+      </c>
+      <c r="B175" t="s">
+        <v>59</v>
+      </c>
+      <c r="C175" t="s">
+        <v>93</v>
+      </c>
+      <c r="D175" t="s">
+        <v>147</v>
+      </c>
+      <c r="E175" t="s">
+        <v>323</v>
+      </c>
+      <c r="F175" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" t="s">
+        <v>60</v>
+      </c>
+      <c r="C176" t="s">
+        <v>88</v>
+      </c>
+      <c r="D176" t="s">
+        <v>148</v>
+      </c>
+      <c r="E176" t="s">
+        <v>324</v>
+      </c>
+      <c r="F176" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" t="s">
+        <v>9</v>
+      </c>
+      <c r="B177" t="s">
+        <v>60</v>
+      </c>
+      <c r="C177" t="s">
+        <v>89</v>
+      </c>
+      <c r="D177" t="s">
+        <v>148</v>
+      </c>
+      <c r="E177" t="s">
+        <v>325</v>
+      </c>
+      <c r="F177" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" t="s">
+        <v>9</v>
+      </c>
+      <c r="B178" t="s">
+        <v>60</v>
+      </c>
+      <c r="C178" t="s">
+        <v>94</v>
+      </c>
+      <c r="D178" t="s">
+        <v>148</v>
+      </c>
+      <c r="E178" t="s">
+        <v>326</v>
+      </c>
+      <c r="F178" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" t="s">
+        <v>9</v>
+      </c>
+      <c r="B179" t="s">
+        <v>60</v>
+      </c>
+      <c r="C179" t="s">
+        <v>95</v>
+      </c>
+      <c r="D179" t="s">
+        <v>148</v>
+      </c>
+      <c r="E179" t="s">
+        <v>327</v>
+      </c>
+      <c r="F179" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" t="s">
+        <v>9</v>
+      </c>
+      <c r="B180" t="s">
+        <v>61</v>
+      </c>
+      <c r="C180" t="s">
+        <v>94</v>
+      </c>
+      <c r="D180" t="s">
+        <v>149</v>
+      </c>
+      <c r="E180" t="s">
+        <v>328</v>
+      </c>
+      <c r="F180" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B181" t="s">
+        <v>61</v>
+      </c>
+      <c r="C181" t="s">
+        <v>95</v>
+      </c>
+      <c r="D181" t="s">
+        <v>149</v>
+      </c>
+      <c r="E181" t="s">
+        <v>329</v>
+      </c>
+      <c r="F181" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" t="s">
+        <v>9</v>
+      </c>
+      <c r="B182" t="s">
+        <v>62</v>
+      </c>
+      <c r="C182" t="s">
+        <v>93</v>
+      </c>
+      <c r="D182" t="s">
+        <v>150</v>
+      </c>
+      <c r="E182" t="s">
+        <v>330</v>
+      </c>
+      <c r="F182" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" t="s">
+        <v>9</v>
+      </c>
+      <c r="B183" t="s">
+        <v>62</v>
+      </c>
+      <c r="C183" t="s">
+        <v>97</v>
+      </c>
+      <c r="D183" t="s">
+        <v>150</v>
+      </c>
+      <c r="E183" t="s">
+        <v>331</v>
+      </c>
+      <c r="F183" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arrumado json para carros
</commit_message>
<xml_diff>
--- a/Fipe_temp.xlsx
+++ b/Fipe_temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="243">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -739,7 +739,7 @@
     <t>008205-8</t>
   </si>
   <si>
-    <t xml:space="preserve"> 143722.00</t>
+    <t xml:space="preserve"> 119187.00</t>
   </si>
   <si>
     <t>junho de 2025</t>
@@ -1100,7 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F350"/>
+  <dimension ref="A1:F351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8099,10 +8099,30 @@
       <c r="D350" t="s">
         <v>240</v>
       </c>
-      <c r="E350" t="s">
+      <c r="E350">
+        <v>143722</v>
+      </c>
+      <c r="F350" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6">
+      <c r="A351" t="s">
+        <v>10</v>
+      </c>
+      <c r="B351" t="s">
+        <v>104</v>
+      </c>
+      <c r="C351" t="s">
+        <v>142</v>
+      </c>
+      <c r="D351" t="s">
+        <v>240</v>
+      </c>
+      <c r="E351" t="s">
         <v>241</v>
       </c>
-      <c r="F350" t="s">
+      <c r="F351" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>